<commit_message>
I decide that Alt1 is so good that I am not going to play around with anything else.
</commit_message>
<xml_diff>
--- a/CH-147 Table Transformation.xlsx
+++ b/CH-147 Table Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCECC1A-394E-49C6-A2A7-C027DA91EA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CD63DB-A41F-4F69-BE7F-D9DAF90034C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="14">
   <si>
     <t>Result</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>logic</t>
+  </si>
+  <si>
+    <t>I think this is the approach I would use going forward.</t>
   </si>
 </sst>
 </file>
@@ -1189,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D8F867-E699-4EA9-86BC-B4C3190A1265}">
   <dimension ref="B1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1379,6 +1382,9 @@
       </c>
       <c r="G12" s="10">
         <v>2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tried to develop and isdate function. Failed
</commit_message>
<xml_diff>
--- a/CH-147 Table Transformation.xlsx
+++ b/CH-147 Table Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CD63DB-A41F-4F69-BE7F-D9DAF90034C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E5D504-B272-4188-962C-ECD4711F632D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1190,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D8F867-E699-4EA9-86BC-B4C3190A1265}">
-  <dimension ref="B1:S40"/>
+  <dimension ref="B1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1990,6 +1990,132 @@
       </c>
       <c r="N40" t="e">
         <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="L42" cm="1">
+        <f t="array" ref="L42:L66">_xlfn.SCAN(, _na, _xlfn.LAMBDA(_xlpm.a,_xlpm.v,IF(ISNUMBER(DATEVALUE(TEXT(_xlpm.v,"dd-mmm-yyyy"))),_xlpm.v,_xlpm.a)))</f>
+        <v>45493</v>
+      </c>
+    </row>
+    <row r="43" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="L43">
+        <v>45493</v>
+      </c>
+    </row>
+    <row r="44" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="L44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="L45">
+        <v>45509</v>
+      </c>
+    </row>
+    <row r="46" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="L46">
+        <v>45509</v>
+      </c>
+    </row>
+    <row r="47" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="L47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="L48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L52">
+        <v>45517</v>
+      </c>
+    </row>
+    <row r="53" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <v>45517</v>
+      </c>
+    </row>
+    <row r="54" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="56" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L56">
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="57" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L62">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="63" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L63">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="64" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L66">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I have decided there is no bulletproof ISDATE function, but the CELL(format) command can be used if the cells have been properly formatted
</commit_message>
<xml_diff>
--- a/CH-147 Table Transformation.xlsx
+++ b/CH-147 Table Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E5D504-B272-4188-962C-ECD4711F632D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E151F531-4A07-4446-BAE0-2D25B3EC6023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="15">
   <si>
     <t>Result</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>I think this is the approach I would use going forward.</t>
+  </si>
+  <si>
+    <t>Cell only tells you the type of cell. It can still contain text.</t>
   </si>
 </sst>
 </file>
@@ -378,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -470,6 +473,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1192,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D8F867-E699-4EA9-86BC-B4C3190A1265}">
   <dimension ref="B1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1248,9 +1254,17 @@
       <c r="G3" s="15">
         <v>10</v>
       </c>
+      <c r="I3" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="I3" ca="1">_xlfn.LAMBDA(_xlpm.d,LEFT(CELL("format",_xlpm.d),1)="D")(C3)</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="J3" ca="1">AND(CELL("format",C3)="D",ISTEXT(C3))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="32" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="5"/>
@@ -1262,6 +1276,14 @@
       </c>
       <c r="G4" s="7">
         <v>8</v>
+      </c>
+      <c r="I4" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="I4" ca="1">_xlfn.LAMBDA(_xlpm.d,LEFT(CELL("format",_xlpm.d),1)="D")(C4)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="J4" ca="1">AND(CELL("format",C4)="D",ISTEXT(C4))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1278,7 +1300,18 @@
       <c r="G5" s="7">
         <v>2</v>
       </c>
+      <c r="I5" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="I5" ca="1">_xlfn.LAMBDA(_xlpm.d,LEFT(CELL("format",_xlpm.d),1)="D")(C5)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="J5" ca="1">AND(CELL("format",C5)="D",ISTEXT(C5))</f>
+        <v>0</v>
+      </c>
       <c r="K5" s="30"/>
+      <c r="L5" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C6" s="25">
@@ -1294,9 +1327,17 @@
       <c r="G6" s="7">
         <v>2</v>
       </c>
+      <c r="I6" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="I6" ca="1">_xlfn.LAMBDA(_xlpm.d,LEFT(CELL("format",_xlpm.d),1)="D")(C6)</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="J6" ca="1">AND(CELL("format",C6)="D",ISTEXT(C6))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="5"/>
@@ -1309,6 +1350,14 @@
       <c r="G7" s="7">
         <v>1</v>
       </c>
+      <c r="I7" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="I7" ca="1">_xlfn.LAMBDA(_xlpm.d,LEFT(CELL("format",_xlpm.d),1)="D")(C7)</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="J7" ca="1">AND(CELL("format",C7)="D",ISTEXT(C7))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C8" s="26">
@@ -1324,9 +1373,13 @@
       <c r="G8" s="18">
         <v>5</v>
       </c>
+      <c r="J8" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="J8" ca="1">AND(CELL("format",C8)="D",ISTEXT(C8))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="32" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="5"/>
@@ -1339,6 +1392,10 @@
       <c r="G9" s="18">
         <v>4</v>
       </c>
+      <c r="J9" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="J9" ca="1">AND(CELL("format",C9)="D",ISTEXT(C9))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C10" s="26">
@@ -1354,9 +1411,13 @@
       <c r="G10" s="18">
         <v>3</v>
       </c>
+      <c r="J10" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="J10" ca="1">AND(CELL("format",C10)="D",ISTEXT(C10))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="32" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="5"/>
@@ -1368,6 +1429,10 @@
       </c>
       <c r="G11" s="7">
         <v>1</v>
+      </c>
+      <c r="J11" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="J11" ca="1">AND(CELL("format",C11)="D",ISTEXT(C11))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
@@ -1393,7 +1458,7 @@
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="32" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1462,7 +1527,7 @@
       </c>
     </row>
     <row r="17" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="32" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
@@ -1532,7 +1597,7 @@
       </c>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="32" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="5">
@@ -1602,7 +1667,7 @@
       </c>
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="32" t="s">
         <v>4</v>
       </c>
       <c r="E21" s="5">
@@ -1707,7 +1772,7 @@
       </c>
     </row>
     <row r="24" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="32" t="s">
         <v>2</v>
       </c>
       <c r="E24" s="5">
@@ -1777,7 +1842,7 @@
       </c>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="32" t="s">
         <v>3</v>
       </c>
       <c r="J26">

</xml_diff>